<commit_message>
Added some methods for parsing/searching imported excel table
</commit_message>
<xml_diff>
--- a/Selenium_project_demo/testData/ClientTestData.xlsx
+++ b/Selenium_project_demo/testData/ClientTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ontariogov-my.sharepoint.com/personal/kyle_o'keeffe_ontario_ca/Documents/Documents/02Projects/ProgProj/OACISTestAutomationSelenium/Data/ExcelImports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ontariogov-my.sharepoint.com/personal/kyle_o'keeffe_ontario_ca/Documents/Documents/02Projects/ProgProj/OACISSeleniumJava/OACIS-Test-Automation-WS/Selenium_project_demo/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="38" documentId="11_F25DC773A252ABDACC104845D9184BC25ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D84924F-A0E6-435C-974E-CF90BEC11D19}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -376,7 +376,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>